<commit_message>
Deploying to gh-pages from @ Healthedata1/USCDI5-Sandbox@c9b217ec1b038b414430d880b3f079f5fe5cde44 🚀
</commit_message>
<xml_diff>
--- a/ValueSet-us-core-adi-finding.xlsx
+++ b/ValueSet-us-core-adi-finding.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>Property</t>
   </si>
@@ -75,6 +75,12 @@
     <t>null (mailto:ehaas@healthedatainc.com)</t>
   </si>
   <si>
+    <t>Jurisdiction</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>Description</t>
   </si>
   <si>
@@ -109,9 +115,6 @@
   </si>
   <si>
     <t>697978002</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>System URI</t>
@@ -251,7 +254,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -353,15 +356,15 @@
       <c r="A12" t="s" s="2">
         <v>22</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" t="s" s="2">
+        <v>23</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>23</v>
-      </c>
-      <c r="B13" t="s" s="2">
         <v>24</v>
       </c>
+      <c r="B13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
@@ -369,6 +372,14 @@
       </c>
       <c r="B14" t="s" s="2">
         <v>26</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="2">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s" s="2">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -390,50 +401,50 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s" s="1">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B5" s="2"/>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>